<commit_message>
Atualização do checklist HD
</commit_message>
<xml_diff>
--- a/docs/Gerenciamento de Projeto/HD - Checklist Verificacao de Projeto.xlsx
+++ b/docs/Gerenciamento de Projeto/HD - Checklist Verificacao de Projeto.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475A8E2F-D29A-4974-A7C6-EF85F006F291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B5F966-D06A-472C-A361-C34BAAB42CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1008,9 +1008,6 @@
     <t>"Referencia não é TAP"</t>
   </si>
   <si>
-    <t>"Esta não é uma restrição"</t>
-  </si>
-  <si>
     <t>Se foi porque não existe o Owner?</t>
   </si>
   <si>
@@ -1018,6 +1015,9 @@
   </si>
   <si>
     <t>Aluisio José Galvão dos Santos (Revisão do projeto Healthy_Delivery)</t>
+  </si>
+  <si>
+    <t>Esta não é uma restrição?</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1541,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.56521739130434778</c:v>
+                  <c:v>0.69565217391304346</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="B3" s="21">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>0.56521739130434778</v>
+        <v>0.69565217391304346</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2088,7 +2088,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2125,7 +2125,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="22">
         <f>COUNTIF(D5:D49,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>0.56521739130434778</v>
+        <v>0.69565217391304346</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1">
@@ -2134,7 +2134,7 @@
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>45</v>
@@ -2241,7 +2241,7 @@
         <v>103</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>124</v>
@@ -2271,10 +2271,10 @@
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F12" s="8"/>
     </row>
@@ -2360,7 +2360,7 @@
         <v>119</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -2537,7 +2537,7 @@
         <v>43</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>123</v>
@@ -2666,7 +2666,7 @@
         <v>119</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F41" s="8"/>
     </row>
@@ -4072,17 +4072,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D10:D12 D14 D8 D16:D49" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -4739,6 +4739,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -4746,11 +4751,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D10:D12 D14 D8 D16:D48" xr:uid="{00000000-0002-0000-0400-000000000000}">

</xml_diff>